<commit_message>
spelling corrections for metadata
</commit_message>
<xml_diff>
--- a/final_data/regen-revisits-metadata.xlsx
+++ b/final_data/regen-revisits-metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tortorec\UCBox\Box Sync\UCDavis\RegenProj\regen-revisits-main\regen-revisits_data\final_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C4BEA5A3-3054-4E63-B517-3E7F3EEC2587}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52541415-0C80-4D75-872D-2D19601B3BE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1A57C630-6931-408B-9F19-A8E215CF3F6F}"/>
   </bookViews>
@@ -200,9 +200,6 @@
     <t>fire incident name</t>
   </si>
   <si>
-    <t xml:space="preserve">fire incident identifyier </t>
-  </si>
-  <si>
     <t>year of fire</t>
   </si>
   <si>
@@ -218,9 +215,6 @@
     <t>Ariel percent cover of hardwoods</t>
   </si>
   <si>
-    <t>heat load calcualted at 30m resolution following McCune &amp; Keon 2002</t>
-  </si>
-  <si>
     <t>LANDFIRE DEM</t>
   </si>
   <si>
@@ -323,10 +317,16 @@
     <t>height of tallest seedling/sapling at the plot (cm)</t>
   </si>
   <si>
-    <t>last year's growth, calcualted as this year's height minus LYHeight (cm)</t>
-  </si>
-  <si>
     <t>last year's height, calculated as height to last budscar (cm)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fire incident identifier </t>
+  </si>
+  <si>
+    <t>heat load calculated at 30m resolution following McCune &amp; Keon 2002</t>
+  </si>
+  <si>
+    <t>last year's growth, calculated as this year's height minus LYHeight (cm)</t>
   </si>
 </sst>
 </file>
@@ -1196,8 +1196,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{076230C7-A640-4DD6-92B4-0092D0A0A973}">
   <dimension ref="A1:C46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1226,7 +1226,7 @@
         <v>48</v>
       </c>
       <c r="C2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -1237,7 +1237,7 @@
         <v>49</v>
       </c>
       <c r="C3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -1248,7 +1248,7 @@
         <v>50</v>
       </c>
       <c r="C4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -1259,7 +1259,7 @@
         <v>51</v>
       </c>
       <c r="C5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -1267,10 +1267,10 @@
         <v>30</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -1281,7 +1281,7 @@
         <v>52</v>
       </c>
       <c r="C7" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -1289,10 +1289,10 @@
         <v>27</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>53</v>
+        <v>93</v>
       </c>
       <c r="C8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -1300,10 +1300,10 @@
         <v>21</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -1311,10 +1311,10 @@
         <v>10</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C10" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -1322,10 +1322,10 @@
         <v>8</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -1333,10 +1333,10 @@
         <v>26</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C12" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -1344,10 +1344,10 @@
         <v>31</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>59</v>
+        <v>94</v>
       </c>
       <c r="C13" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
@@ -1355,10 +1355,10 @@
         <v>22</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C14" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -1366,10 +1366,10 @@
         <v>39</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C15" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
@@ -1377,10 +1377,10 @@
         <v>38</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C16" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
@@ -1388,10 +1388,10 @@
         <v>44</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C17" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
@@ -1399,10 +1399,10 @@
         <v>16</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C18" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
@@ -1410,10 +1410,10 @@
         <v>17</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C19" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
@@ -1421,10 +1421,10 @@
         <v>7</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C20" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
@@ -1432,10 +1432,10 @@
         <v>18</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C21" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -1443,10 +1443,10 @@
         <v>35</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C22" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -1454,10 +1454,10 @@
         <v>3</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C23" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
@@ -1465,10 +1465,10 @@
         <v>2</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C24" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
@@ -1476,10 +1476,10 @@
         <v>33</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C25" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
@@ -1487,10 +1487,10 @@
         <v>43</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C26" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
@@ -1498,10 +1498,10 @@
         <v>28</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C27" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
@@ -1509,10 +1509,10 @@
         <v>4</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C28" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
@@ -1520,10 +1520,10 @@
         <v>20</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C29" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
@@ -1531,10 +1531,10 @@
         <v>42</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C30" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
@@ -1542,10 +1542,10 @@
         <v>14</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C31" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
@@ -1553,10 +1553,10 @@
         <v>15</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C32" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
@@ -1564,10 +1564,10 @@
         <v>25</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C33" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
@@ -1575,10 +1575,10 @@
         <v>9</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C34" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
@@ -1586,10 +1586,10 @@
         <v>13</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C35" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
@@ -1597,10 +1597,10 @@
         <v>5</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C36" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
@@ -1608,10 +1608,10 @@
         <v>40</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C37" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -1619,10 +1619,10 @@
         <v>41</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C38" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
@@ -1630,10 +1630,10 @@
         <v>24</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C39" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
@@ -1641,10 +1641,10 @@
         <v>29</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C40" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
@@ -1652,10 +1652,10 @@
         <v>37</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C41" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
@@ -1663,10 +1663,10 @@
         <v>32</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C42" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -1674,10 +1674,10 @@
         <v>12</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C43" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
@@ -1685,10 +1685,10 @@
         <v>1</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C44" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
@@ -1696,10 +1696,10 @@
         <v>34</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C45" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
@@ -1707,10 +1707,10 @@
         <v>23</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C46" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>